<commit_message>
data analysis in jupyter notebook
- data analysis
- sort of columns
</commit_message>
<xml_diff>
--- a/data-visualization/power-bi/examples/sorting-tables/data/prod_data3.xlsx
+++ b/data-visualization/power-bi/examples/sorting-tables/data/prod_data3.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Quality Index</t>
   </si>
   <si>
-    <t xml:space="preserve">Apple 1</t>
+    <t xml:space="preserve">Apple1</t>
   </si>
   <si>
     <t xml:space="preserve">Apple2</t>
@@ -352,7 +352,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>